<commit_message>
cambie graph a plotly express
</commit_message>
<xml_diff>
--- a/src/data/experimento.xlsx
+++ b/src/data/experimento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Python_Source_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\PY_TEST\Test01_render\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{109BF629-AC16-4B6A-836C-31226E0CAB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E85C0F8-D891-42F5-916B-D912723ADBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DF2E6045-9878-4AFA-A5FB-FF5DCBB8EC95}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DF2E6045-9878-4AFA-A5FB-FF5DCBB8EC95}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -220,9 +220,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -260,7 +260,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -366,7 +366,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -508,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -523,6 +523,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>